<commit_message>
Implementacion BBDD, queda refactor + exporte
</commit_message>
<xml_diff>
--- a/build/classes/resources/SistemasAgua.xlsx
+++ b/build/classes/resources/SistemasAgua.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354412" uniqueCount="880">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24252" uniqueCount="878">
   <si>
     <t>Nombre</t>
   </si>
@@ -2363,12 +2363,6 @@
   </si>
   <si>
     <t>15/01/2011</t>
-  </si>
-  <si>
-    <t>20012541150023365233</t>
-  </si>
-  <si>
-    <t>FR3820012541150023365233</t>
   </si>
   <si>
     <t>801.0</t>
@@ -6598,11 +6592,9 @@
         <v>376</v>
       </c>
       <c r="H83" t="s" s="0">
-        <v>779</v>
-      </c>
-      <c r="I83" t="s" s="0">
-        <v>780</v>
-      </c>
+        <v>335</v>
+      </c>
+      <c r="I83" s="0"/>
       <c r="J83" s="0"/>
       <c r="K83" t="s" s="0">
         <v>264</v>
@@ -6611,13 +6603,13 @@
         <v>510</v>
       </c>
       <c r="M83" t="s" s="0">
+        <v>779</v>
+      </c>
+      <c r="N83" t="s" s="0">
+        <v>780</v>
+      </c>
+      <c r="O83" t="s" s="7">
         <v>781</v>
-      </c>
-      <c r="N83" t="s" s="0">
-        <v>782</v>
-      </c>
-      <c r="O83" t="s" s="7">
-        <v>783</v>
       </c>
       <c r="P83" s="0"/>
       <c r="Q83" t="s" s="1">
@@ -6648,7 +6640,7 @@
         <v>336</v>
       </c>
       <c r="I84" t="s" s="0">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="J84" s="0"/>
       <c r="K84" t="s" s="0">
@@ -6658,13 +6650,13 @@
         <v>510</v>
       </c>
       <c r="M84" t="s" s="0">
+        <v>783</v>
+      </c>
+      <c r="N84" t="s" s="0">
+        <v>784</v>
+      </c>
+      <c r="O84" t="s" s="7">
         <v>785</v>
-      </c>
-      <c r="N84" t="s" s="0">
-        <v>786</v>
-      </c>
-      <c r="O84" t="s" s="7">
-        <v>787</v>
       </c>
       <c r="P84" s="0"/>
       <c r="Q84" t="s" s="1">
@@ -6698,7 +6690,7 @@
         <v>337</v>
       </c>
       <c r="I86" t="s" s="0">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="J86" s="0"/>
       <c r="K86" t="s" s="0">
@@ -6708,13 +6700,13 @@
         <v>523</v>
       </c>
       <c r="M86" t="s" s="0">
+        <v>787</v>
+      </c>
+      <c r="N86" t="s" s="0">
+        <v>788</v>
+      </c>
+      <c r="O86" t="s" s="7">
         <v>789</v>
-      </c>
-      <c r="N86" t="s" s="0">
-        <v>790</v>
-      </c>
-      <c r="O86" t="s" s="7">
-        <v>791</v>
       </c>
       <c r="P86" s="0"/>
       <c r="Q86" t="s" s="1">
@@ -6747,7 +6739,7 @@
         <v>338</v>
       </c>
       <c r="I87" t="s" s="0">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="J87" s="0"/>
       <c r="K87" t="s" s="0">
@@ -6757,13 +6749,13 @@
         <v>510</v>
       </c>
       <c r="M87" t="s" s="0">
+        <v>791</v>
+      </c>
+      <c r="N87" t="s" s="0">
+        <v>792</v>
+      </c>
+      <c r="O87" t="s" s="7">
         <v>793</v>
-      </c>
-      <c r="N87" t="s" s="0">
-        <v>794</v>
-      </c>
-      <c r="O87" t="s" s="7">
-        <v>795</v>
       </c>
       <c r="P87" s="0"/>
       <c r="Q87" t="s" s="1">
@@ -6796,7 +6788,7 @@
         <v>339</v>
       </c>
       <c r="I88" t="s" s="0">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="J88" s="0"/>
       <c r="K88" t="s" s="0">
@@ -6806,13 +6798,13 @@
         <v>510</v>
       </c>
       <c r="M88" t="s" s="0">
+        <v>795</v>
+      </c>
+      <c r="N88" t="s" s="0">
+        <v>796</v>
+      </c>
+      <c r="O88" t="s" s="7">
         <v>797</v>
-      </c>
-      <c r="N88" t="s" s="0">
-        <v>798</v>
-      </c>
-      <c r="O88" t="s" s="7">
-        <v>799</v>
       </c>
       <c r="P88" s="0"/>
       <c r="Q88" t="s" s="1">
@@ -6845,7 +6837,7 @@
         <v>340</v>
       </c>
       <c r="I89" t="s" s="0">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J89" s="0"/>
       <c r="K89" t="s" s="0">
@@ -6858,10 +6850,10 @@
         <v>773</v>
       </c>
       <c r="N89" t="s" s="0">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="O89" t="s" s="7">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="P89" s="0"/>
       <c r="Q89" t="s" s="1">
@@ -6900,13 +6892,13 @@
         <v>510</v>
       </c>
       <c r="M90" t="s" s="0">
+        <v>801</v>
+      </c>
+      <c r="N90" t="s" s="0">
+        <v>802</v>
+      </c>
+      <c r="O90" t="s" s="7">
         <v>803</v>
-      </c>
-      <c r="N90" t="s" s="0">
-        <v>804</v>
-      </c>
-      <c r="O90" t="s" s="7">
-        <v>805</v>
       </c>
       <c r="P90" s="0"/>
       <c r="Q90" t="s" s="1">
@@ -6939,7 +6931,7 @@
         <v>342</v>
       </c>
       <c r="I91" t="s" s="0">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="J91" s="0"/>
       <c r="K91" t="s" s="0">
@@ -6949,13 +6941,13 @@
         <v>510</v>
       </c>
       <c r="M91" t="s" s="0">
+        <v>805</v>
+      </c>
+      <c r="N91" t="s" s="0">
+        <v>806</v>
+      </c>
+      <c r="O91" t="s" s="7">
         <v>807</v>
-      </c>
-      <c r="N91" t="s" s="0">
-        <v>808</v>
-      </c>
-      <c r="O91" t="s" s="7">
-        <v>809</v>
       </c>
       <c r="P91" s="0"/>
       <c r="Q91" t="s" s="1">
@@ -6988,7 +6980,7 @@
         <v>343</v>
       </c>
       <c r="I92" t="s" s="0">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="J92" s="0"/>
       <c r="K92" t="s" s="0">
@@ -6998,13 +6990,13 @@
         <v>510</v>
       </c>
       <c r="M92" t="s" s="0">
-        <v>811</v>
+        <v>809</v>
       </c>
       <c r="N92" t="s" s="0">
         <v>612</v>
       </c>
       <c r="O92" t="s" s="7">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="P92" s="0"/>
       <c r="Q92" t="s" s="1">
@@ -7037,7 +7029,7 @@
         <v>344</v>
       </c>
       <c r="I93" t="s" s="0">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="J93" s="0"/>
       <c r="K93" t="s" s="0">
@@ -7047,13 +7039,13 @@
         <v>523</v>
       </c>
       <c r="M93" t="s" s="0">
+        <v>812</v>
+      </c>
+      <c r="N93" t="s" s="0">
+        <v>813</v>
+      </c>
+      <c r="O93" t="s" s="7">
         <v>814</v>
-      </c>
-      <c r="N93" t="s" s="0">
-        <v>815</v>
-      </c>
-      <c r="O93" t="s" s="7">
-        <v>816</v>
       </c>
       <c r="P93" s="0"/>
       <c r="Q93" t="s" s="1">
@@ -7092,13 +7084,13 @@
         <v>510</v>
       </c>
       <c r="M94" t="s" s="0">
+        <v>815</v>
+      </c>
+      <c r="N94" t="s" s="0">
+        <v>816</v>
+      </c>
+      <c r="O94" t="s" s="7">
         <v>817</v>
-      </c>
-      <c r="N94" t="s" s="0">
-        <v>818</v>
-      </c>
-      <c r="O94" t="s" s="7">
-        <v>819</v>
       </c>
       <c r="P94" s="0"/>
       <c r="Q94" t="s" s="1">
@@ -7131,7 +7123,7 @@
         <v>346</v>
       </c>
       <c r="I95" t="s" s="0">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="J95" s="0"/>
       <c r="K95" t="s" s="0">
@@ -7141,13 +7133,13 @@
         <v>510</v>
       </c>
       <c r="M95" t="s" s="0">
+        <v>819</v>
+      </c>
+      <c r="N95" t="s" s="0">
+        <v>820</v>
+      </c>
+      <c r="O95" t="s" s="7">
         <v>821</v>
-      </c>
-      <c r="N95" t="s" s="0">
-        <v>822</v>
-      </c>
-      <c r="O95" t="s" s="7">
-        <v>823</v>
       </c>
       <c r="P95" s="0"/>
       <c r="Q95" t="s" s="1">
@@ -7183,10 +7175,10 @@
         <v>373</v>
       </c>
       <c r="H102" t="s" s="0">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="I102" t="s" s="0">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="J102" s="0"/>
       <c r="K102" t="s" s="0">
@@ -7196,13 +7188,13 @@
         <v>510</v>
       </c>
       <c r="M102" t="s" s="0">
+        <v>824</v>
+      </c>
+      <c r="N102" t="s" s="0">
+        <v>825</v>
+      </c>
+      <c r="O102" t="s" s="7">
         <v>826</v>
-      </c>
-      <c r="N102" t="s" s="0">
-        <v>827</v>
-      </c>
-      <c r="O102" t="s" s="7">
-        <v>828</v>
       </c>
       <c r="P102" s="0"/>
       <c r="Q102" t="s" s="1">
@@ -7232,10 +7224,10 @@
         <v>374</v>
       </c>
       <c r="H103" t="s" s="0">
-        <v>829</v>
+        <v>827</v>
       </c>
       <c r="I103" t="s" s="0">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="J103" s="0"/>
       <c r="K103" t="s" s="0">
@@ -7245,13 +7237,13 @@
         <v>523</v>
       </c>
       <c r="M103" t="s" s="0">
+        <v>829</v>
+      </c>
+      <c r="N103" t="s" s="0">
+        <v>830</v>
+      </c>
+      <c r="O103" t="s" s="7">
         <v>831</v>
-      </c>
-      <c r="N103" t="s" s="0">
-        <v>832</v>
-      </c>
-      <c r="O103" t="s" s="7">
-        <v>833</v>
       </c>
       <c r="P103" s="0"/>
       <c r="Q103" t="s" s="1">
@@ -7284,7 +7276,7 @@
         <v>349</v>
       </c>
       <c r="I104" t="s" s="0">
-        <v>834</v>
+        <v>832</v>
       </c>
       <c r="J104" s="0"/>
       <c r="K104" t="s" s="0">
@@ -7297,10 +7289,10 @@
         <v>558</v>
       </c>
       <c r="N104" t="s" s="0">
-        <v>835</v>
+        <v>833</v>
       </c>
       <c r="O104" t="s" s="7">
-        <v>836</v>
+        <v>834</v>
       </c>
       <c r="P104" s="0"/>
       <c r="Q104" t="s" s="1">
@@ -7341,13 +7333,13 @@
         <v>510</v>
       </c>
       <c r="M105" t="s" s="0">
+        <v>835</v>
+      </c>
+      <c r="N105" t="s" s="0">
+        <v>836</v>
+      </c>
+      <c r="O105" t="s" s="7">
         <v>837</v>
-      </c>
-      <c r="N105" t="s" s="0">
-        <v>838</v>
-      </c>
-      <c r="O105" t="s" s="7">
-        <v>839</v>
       </c>
       <c r="P105" s="0"/>
       <c r="Q105" t="s" s="1">
@@ -7377,10 +7369,10 @@
         <v>381</v>
       </c>
       <c r="H106" t="s" s="0">
-        <v>840</v>
+        <v>838</v>
       </c>
       <c r="I106" t="s" s="0">
-        <v>841</v>
+        <v>839</v>
       </c>
       <c r="J106" s="0"/>
       <c r="K106" t="s" s="0">
@@ -7390,13 +7382,13 @@
         <v>523</v>
       </c>
       <c r="M106" t="s" s="0">
+        <v>840</v>
+      </c>
+      <c r="N106" t="s" s="0">
+        <v>841</v>
+      </c>
+      <c r="O106" t="s" s="7">
         <v>842</v>
-      </c>
-      <c r="N106" t="s" s="0">
-        <v>843</v>
-      </c>
-      <c r="O106" t="s" s="7">
-        <v>844</v>
       </c>
       <c r="P106" s="0"/>
       <c r="Q106" t="s" s="1">
@@ -7457,13 +7449,13 @@
         <v>510</v>
       </c>
       <c r="M127" t="s" s="0">
+        <v>843</v>
+      </c>
+      <c r="N127" t="s" s="0">
+        <v>844</v>
+      </c>
+      <c r="O127" t="s" s="7">
         <v>845</v>
-      </c>
-      <c r="N127" t="s" s="0">
-        <v>846</v>
-      </c>
-      <c r="O127" t="s" s="7">
-        <v>847</v>
       </c>
       <c r="P127" s="0"/>
       <c r="Q127" t="s" s="1">
@@ -7493,10 +7485,10 @@
         <v>369</v>
       </c>
       <c r="H128" t="s" s="0">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="I128" t="s" s="0">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="J128" s="0"/>
       <c r="K128" t="s" s="0">
@@ -7506,13 +7498,13 @@
         <v>510</v>
       </c>
       <c r="M128" t="s" s="0">
+        <v>848</v>
+      </c>
+      <c r="N128" t="s" s="0">
+        <v>849</v>
+      </c>
+      <c r="O128" t="s" s="7">
         <v>850</v>
-      </c>
-      <c r="N128" t="s" s="0">
-        <v>851</v>
-      </c>
-      <c r="O128" t="s" s="7">
-        <v>852</v>
       </c>
       <c r="P128" s="0"/>
       <c r="Q128" t="s" s="1">
@@ -7545,7 +7537,7 @@
         <v>354</v>
       </c>
       <c r="I129" t="s" s="0">
-        <v>853</v>
+        <v>851</v>
       </c>
       <c r="J129" s="0"/>
       <c r="K129" t="s" s="0">
@@ -7555,13 +7547,13 @@
         <v>510</v>
       </c>
       <c r="M129" t="s" s="0">
+        <v>852</v>
+      </c>
+      <c r="N129" t="s" s="0">
+        <v>853</v>
+      </c>
+      <c r="O129" t="s" s="7">
         <v>854</v>
-      </c>
-      <c r="N129" t="s" s="0">
-        <v>855</v>
-      </c>
-      <c r="O129" t="s" s="7">
-        <v>856</v>
       </c>
       <c r="P129" s="0"/>
       <c r="Q129" t="s" s="1">
@@ -7602,13 +7594,13 @@
         <v>523</v>
       </c>
       <c r="M130" t="s" s="0">
-        <v>857</v>
+        <v>855</v>
       </c>
       <c r="N130" t="s" s="0">
         <v>634</v>
       </c>
       <c r="O130" t="s" s="7">
-        <v>858</v>
+        <v>856</v>
       </c>
       <c r="P130" s="0"/>
       <c r="Q130" t="s" s="1">
@@ -7641,7 +7633,7 @@
         <v>356</v>
       </c>
       <c r="I131" t="s" s="0">
-        <v>859</v>
+        <v>857</v>
       </c>
       <c r="J131" s="0"/>
       <c r="K131" t="s" s="0">
@@ -7651,13 +7643,13 @@
         <v>510</v>
       </c>
       <c r="M131" t="s" s="0">
+        <v>858</v>
+      </c>
+      <c r="N131" t="s" s="0">
+        <v>859</v>
+      </c>
+      <c r="O131" t="s" s="7">
         <v>860</v>
-      </c>
-      <c r="N131" t="s" s="0">
-        <v>861</v>
-      </c>
-      <c r="O131" t="s" s="7">
-        <v>862</v>
       </c>
       <c r="P131" s="0"/>
       <c r="Q131" t="s" s="1">
@@ -7690,7 +7682,7 @@
         <v>357</v>
       </c>
       <c r="I132" t="s" s="0">
-        <v>863</v>
+        <v>861</v>
       </c>
       <c r="J132" s="0"/>
       <c r="K132" t="s" s="0">
@@ -7700,13 +7692,13 @@
         <v>510</v>
       </c>
       <c r="M132" t="s" s="0">
+        <v>862</v>
+      </c>
+      <c r="N132" t="s" s="0">
+        <v>863</v>
+      </c>
+      <c r="O132" t="s" s="7">
         <v>864</v>
-      </c>
-      <c r="N132" t="s" s="0">
-        <v>865</v>
-      </c>
-      <c r="O132" t="s" s="7">
-        <v>866</v>
       </c>
       <c r="P132" s="0"/>
       <c r="Q132" t="s" s="1">
@@ -7739,7 +7731,7 @@
         <v>358</v>
       </c>
       <c r="I133" t="s" s="0">
-        <v>867</v>
+        <v>865</v>
       </c>
       <c r="J133" s="0"/>
       <c r="K133" t="s" s="0">
@@ -7749,13 +7741,13 @@
         <v>510</v>
       </c>
       <c r="M133" t="s" s="0">
+        <v>866</v>
+      </c>
+      <c r="N133" t="s" s="0">
+        <v>867</v>
+      </c>
+      <c r="O133" t="s" s="7">
         <v>868</v>
-      </c>
-      <c r="N133" t="s" s="0">
-        <v>869</v>
-      </c>
-      <c r="O133" t="s" s="7">
-        <v>870</v>
       </c>
       <c r="P133" s="0"/>
       <c r="Q133" t="s" s="1">
@@ -7788,7 +7780,7 @@
         <v>359</v>
       </c>
       <c r="I134" t="s" s="0">
-        <v>871</v>
+        <v>869</v>
       </c>
       <c r="J134" s="0"/>
       <c r="K134" t="s" s="0">
@@ -7798,13 +7790,13 @@
         <v>523</v>
       </c>
       <c r="M134" t="s" s="0">
-        <v>872</v>
+        <v>870</v>
       </c>
       <c r="N134" t="s" s="0">
         <v>770</v>
       </c>
       <c r="O134" t="s" s="7">
-        <v>873</v>
+        <v>871</v>
       </c>
       <c r="P134" s="0"/>
       <c r="Q134" t="s" s="1">
@@ -7843,13 +7835,13 @@
         <v>510</v>
       </c>
       <c r="M135" t="s" s="0">
+        <v>872</v>
+      </c>
+      <c r="N135" t="s" s="0">
+        <v>873</v>
+      </c>
+      <c r="O135" t="s" s="7">
         <v>874</v>
-      </c>
-      <c r="N135" t="s" s="0">
-        <v>875</v>
-      </c>
-      <c r="O135" t="s" s="7">
-        <v>876</v>
       </c>
       <c r="P135" s="0"/>
       <c r="Q135" t="s" s="1">
@@ -7882,7 +7874,7 @@
         <v>361</v>
       </c>
       <c r="I136" t="s" s="0">
-        <v>877</v>
+        <v>875</v>
       </c>
       <c r="J136" s="0"/>
       <c r="K136" t="s" s="0">
@@ -7892,13 +7884,13 @@
         <v>510</v>
       </c>
       <c r="M136" t="s" s="0">
-        <v>878</v>
+        <v>876</v>
       </c>
       <c r="N136" t="s" s="0">
         <v>650</v>
       </c>
       <c r="O136" t="s" s="7">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="P136" s="0"/>
       <c r="Q136" t="s" s="1">

</xml_diff>